<commit_message>
removed hospital class and changed the printing style
</commit_message>
<xml_diff>
--- a/db/DOCTOR.xlsx
+++ b/db/DOCTOR.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,34 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>kushal@krishanppa.practo</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['Surgeon']</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0123456789</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
removed hospital db, added values to doctor db
</commit_message>
<xml_diff>
--- a/db/DOCTOR.xlsx
+++ b/db/DOCTOR.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,26 +468,222 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>kushal@krishanppa.practo</t>
+          <t>shailesh@prac.to</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>['Dermatologist']</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>9087654321</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>uthappa@prac.to</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['Cardiologist']</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>9087654321</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sheela@prac.to</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['Dermatologist']</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>9087654321</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>uthmini@prac.to</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['Cardiologist']</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>9087654321</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>raj@prac.to</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['General']</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>20</v>
+      </c>
+      <c r="D6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>9087654321</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rajani@prac.to</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>['General']</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>19</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>9087654321</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>pulasthya@prac.to</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>['Surgeon']</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C8" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0123456789</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>9087654321</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Pulsathi@prac.to</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>['Surgeon']</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>9087654321</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>N</t>
         </is>

</xml_diff>